<commit_message>
coed for style in dashboard. done 1st stage
</commit_message>
<xml_diff>
--- a/EFI/CODE/input/anagrafiche/rf2supergroup.xlsx
+++ b/EFI/CODE/input/anagrafiche/rf2supergroup.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u093799\Desktop\EFI\CODE\input\anagrafiche\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\u093799\Documents\GitHub\PrimoRepository\EFI\CODE\input\anagrafiche\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEAACF86-70D9-4F4C-ACF1-B44D37A48515}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="18825" windowHeight="7200"/>
+    <workbookView xWindow="1455" yWindow="0" windowWidth="19035" windowHeight="11520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
     <sheet name="rf32" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,6 +24,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -311,7 +315,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -700,11 +704,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="A2" sqref="A2:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -729,346 +733,346 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>1</v>
+        <v>67</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>2</v>
+        <v>68</v>
       </c>
       <c r="D2" s="5">
-        <v>9.0909090909090912E-2</v>
+        <v>7.6923076923076927E-2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>3</v>
+        <v>69</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>1</v>
+        <v>67</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>2</v>
+        <v>68</v>
       </c>
       <c r="D3" s="5">
-        <v>9.0909090909090912E-2</v>
+        <v>7.6923076923076927E-2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>4</v>
+        <v>70</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>1</v>
+        <v>67</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>2</v>
+        <v>68</v>
       </c>
       <c r="D4" s="5">
-        <v>9.0909090909090912E-2</v>
+        <v>7.6923076923076927E-2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>5</v>
+        <v>71</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>1</v>
+        <v>67</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>2</v>
+        <v>68</v>
       </c>
       <c r="D5" s="5">
-        <v>9.0909090909090912E-2</v>
+        <v>7.6923076923076927E-2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>6</v>
+        <v>72</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>7</v>
+        <v>73</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>2</v>
+        <v>68</v>
       </c>
       <c r="D6" s="5">
-        <v>9.0909090909090912E-2</v>
+        <v>7.6923076923076927E-2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>9</v>
+        <v>73</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>2</v>
+        <v>68</v>
       </c>
       <c r="D7" s="5">
-        <v>9.0909090909090912E-2</v>
+        <v>7.6923076923076927E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>10</v>
+        <v>75</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>9</v>
+        <v>73</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>2</v>
+        <v>68</v>
       </c>
       <c r="D8" s="5">
-        <v>9.0909090909090912E-2</v>
+        <v>7.6923076923076927E-2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>11</v>
+        <v>76</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>12</v>
+        <v>73</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>2</v>
+        <v>68</v>
       </c>
       <c r="D9" s="5">
-        <v>9.0909090909090912E-2</v>
+        <v>7.6923076923076927E-2</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>13</v>
+        <v>77</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>14</v>
+        <v>78</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>2</v>
+        <v>68</v>
       </c>
       <c r="D10" s="5">
-        <v>9.0909090909090912E-2</v>
+        <v>7.6923076923076927E-2</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>14</v>
+        <v>80</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>2</v>
+        <v>68</v>
       </c>
       <c r="D11" s="5">
-        <v>9.0909090909090912E-2</v>
+        <v>7.6923076923076927E-2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>16</v>
+        <v>81</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>17</v>
+        <v>82</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>2</v>
+        <v>68</v>
       </c>
       <c r="D12" s="5">
-        <v>9.0909090909090912E-2</v>
+        <v>7.6923076923076927E-2</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>18</v>
+        <v>83</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="D13" s="5">
-        <v>5.5555555555555552E-2</v>
+        <v>7.6923076923076927E-2</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>20</v>
+        <v>89</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>21</v>
+        <v>83</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="D14" s="5">
-        <v>5.5555555555555552E-2</v>
+        <v>7.6923076923076927E-2</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="D15" s="5">
-        <v>5.5555555555555552E-2</v>
+        <v>9.0909090909090912E-2</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="D16" s="5">
-        <v>5.5555555555555552E-2</v>
+        <v>9.0909090909090912E-2</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="D17" s="5">
-        <v>5.5555555555555552E-2</v>
+        <v>9.0909090909090912E-2</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="D18" s="5">
-        <v>5.5555555555555552E-2</v>
+        <v>9.0909090909090912E-2</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="D19" s="5">
-        <v>5.5555555555555552E-2</v>
+        <v>9.0909090909090912E-2</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="D20" s="5">
-        <v>5.5555555555555552E-2</v>
+        <v>9.0909090909090912E-2</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="D21" s="5">
-        <v>5.5555555555555552E-2</v>
+        <v>9.0909090909090912E-2</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="D22" s="5">
-        <v>5.5555555555555552E-2</v>
+        <v>9.0909090909090912E-2</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="D23" s="5">
-        <v>5.5555555555555552E-2</v>
+        <v>9.0909090909090912E-2</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="D24" s="5">
-        <v>5.5555555555555552E-2</v>
+        <v>9.0909090909090912E-2</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="D25" s="5">
-        <v>5.5555555555555552E-2</v>
+        <v>9.0909090909090912E-2</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>36</v>
+        <v>87</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>19</v>
@@ -1079,10 +1083,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>19</v>
@@ -1093,10 +1097,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>19</v>
@@ -1107,10 +1111,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>19</v>
@@ -1121,10 +1125,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>19</v>
@@ -1135,192 +1139,192 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="D31" s="5">
-        <v>6.25E-2</v>
+        <v>5.5555555555555552E-2</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="D32" s="5">
-        <v>6.25E-2</v>
+        <v>5.5555555555555552E-2</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="D33" s="5">
-        <v>6.25E-2</v>
+        <v>5.5555555555555552E-2</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="D34" s="5">
-        <v>6.25E-2</v>
+        <v>5.5555555555555552E-2</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="D35" s="5">
-        <v>6.25E-2</v>
+        <v>5.5555555555555552E-2</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="D36" s="5">
-        <v>6.25E-2</v>
+        <v>5.5555555555555552E-2</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="D37" s="5">
-        <v>6.25E-2</v>
+        <v>5.5555555555555552E-2</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="D38" s="5">
-        <v>6.25E-2</v>
+        <v>5.5555555555555552E-2</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="D39" s="5">
-        <v>6.25E-2</v>
+        <v>5.5555555555555552E-2</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="D40" s="5">
-        <v>6.25E-2</v>
+        <v>5.5555555555555552E-2</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="D41" s="5">
-        <v>6.25E-2</v>
+        <v>5.5555555555555552E-2</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="D42" s="5">
-        <v>6.25E-2</v>
+        <v>5.5555555555555552E-2</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="D43" s="5">
-        <v>6.25E-2</v>
+        <v>5.5555555555555552E-2</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>43</v>
@@ -1331,10 +1335,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>43</v>
@@ -1345,10 +1349,10 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>43</v>
@@ -1359,184 +1363,184 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="D47" s="5">
-        <v>7.6923076923076927E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="D48" s="5">
-        <v>7.6923076923076927E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="D49" s="5">
-        <v>7.6923076923076927E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="D50" s="5">
-        <v>7.6923076923076927E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="D51" s="5">
-        <v>7.6923076923076927E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="D52" s="5">
-        <v>7.6923076923076927E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="D53" s="5">
-        <v>7.6923076923076927E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="D54" s="5">
-        <v>7.6923076923076927E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="D55" s="5">
-        <v>7.6923076923076927E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="D56" s="5">
-        <v>7.6923076923076927E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="D57" s="5">
-        <v>7.6923076923076927E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>88</v>
+        <v>62</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="D58" s="5">
-        <v>7.6923076923076927E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="D59" s="5">
-        <v>7.6923076923076927E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1546,7 +1550,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A33"/>
   <sheetViews>
     <sheetView topLeftCell="A15" workbookViewId="0">

</xml_diff>